<commit_message>
Problems with postalCode, workarounds
postalCode is throwing errors on some queries. I'm thinking it might be because the field is empty on some records. I tried going back to the original code to figure out how to add error checking. Created a new "ebaysdk_test" using the sdk's sample code.
</commit_message>
<xml_diff>
--- a/Results_leslie_solid_state.xlsx
+++ b/Results_leslie_solid_state.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
   <si>
     <t>itemId</t>
   </si>
@@ -23,7 +23,7 @@
     <t>title</t>
   </si>
   <si>
-    <t>condition</t>
+    <t>conditionDisplayName</t>
   </si>
   <si>
     <t>currentPrice</t>
@@ -59,42 +59,90 @@
     <t>postalCode</t>
   </si>
   <si>
+    <t>galleryURL</t>
+  </si>
+  <si>
     <t>viewItemURL</t>
   </si>
   <si>
+    <t>sellerUserName</t>
+  </si>
+  <si>
+    <t>feedbackScore</t>
+  </si>
+  <si>
+    <t>positiveFeedbackPercent</t>
+  </si>
+  <si>
+    <t>282979136920</t>
+  </si>
+  <si>
+    <t>Leslie 760 Speaker connected to Hammond M3</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>EndedWithoutSales</t>
+  </si>
+  <si>
+    <t>FixedPrice</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Columbus,OH,USA</t>
+  </si>
+  <si>
+    <t>43219</t>
+  </si>
+  <si>
+    <t>http://thumbs1.ebaystatic.com/m/mcW56GTxJ8mOuVTfJV5PXsA/140.jpg</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/Leslie-760-Speaker-connected-Hammond-M3-/282979136920</t>
+  </si>
+  <si>
+    <t>retro-cool1969</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
     <t>153056191662</t>
   </si>
   <si>
     <t>Leslie Speaker Model 825</t>
   </si>
   <si>
-    <t>Used</t>
-  </si>
-  <si>
-    <t>EndedWithoutSales</t>
-  </si>
-  <si>
     <t>StoreInventory</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>2018-06-09T21:15:11.000Z</t>
-  </si>
-  <si>
-    <t>2018-06-19T21:15:11.000Z</t>
-  </si>
-  <si>
     <t>Upland,CA,USA</t>
   </si>
   <si>
+    <t>91786</t>
+  </si>
+  <si>
+    <t>http://thumbs3.ebaystatic.com/m/maoyr85am-Mw8sEDWZIBQTQ/140.jpg</t>
+  </si>
+  <si>
     <t>http://www.ebay.com/itm/Leslie-Speaker-Model-825-/153056191662</t>
   </si>
   <si>
+    <t>electronics7111</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
     <t>202311640461</t>
   </si>
   <si>
@@ -107,45 +155,33 @@
     <t>EndedWithSales</t>
   </si>
   <si>
-    <t>FixedPrice</t>
-  </si>
-  <si>
-    <t>2018-05-12T17:42:54.000Z</t>
-  </si>
-  <si>
-    <t>2018-06-05T20:09:31.000Z</t>
-  </si>
-  <si>
     <t>Pawtucket,RI,USA</t>
   </si>
   <si>
+    <t>02861</t>
+  </si>
+  <si>
+    <t>http://thumbs2.ebaystatic.com/m/m-c-JbCQeOXIWZCdikSCoBw/140.jpg</t>
+  </si>
+  <si>
     <t>http://www.ebay.com/itm/combo-preamp-leslie-amp-9-pins-700-710-760-770-825-830-900-910-925-950-series-/202311640461</t>
   </si>
   <si>
+    <t>moe-foe_greenwing</t>
+  </si>
+  <si>
+    <t>1909</t>
+  </si>
+  <si>
     <t>153036533548</t>
   </si>
   <si>
-    <t>2018-05-25T15:50:32.000Z</t>
-  </si>
-  <si>
-    <t>2018-06-04T15:50:32.000Z</t>
+    <t>http://thumbs1.ebaystatic.com/m/maoyr85am-Mw8sEDWZIBQTQ/140.jpg</t>
   </si>
   <si>
     <t>http://www.ebay.com/itm/Leslie-Speaker-Model-825-/153036533548</t>
   </si>
   <si>
-    <t>163047650069</t>
-  </si>
-  <si>
-    <t>2018-05-14T19:25:58.000Z</t>
-  </si>
-  <si>
-    <t>2018-05-24T19:25:58.000Z</t>
-  </si>
-  <si>
-    <t>http://www.ebay.com/itm/Leslie-Speaker-Model-825-/163047650069</t>
-  </si>
-  <si>
     <t>142783280008</t>
   </si>
   <si>
@@ -155,59 +191,80 @@
     <t>Auction</t>
   </si>
   <si>
-    <t>2018-05-05T00:58:47.000Z</t>
-  </si>
-  <si>
-    <t>2018-05-05T01:08:22.000Z</t>
-  </si>
-  <si>
     <t>Collingswood,NJ,USA</t>
   </si>
   <si>
+    <t>08108</t>
+  </si>
+  <si>
+    <t>http://thumbs1.ebaystatic.com/m/mzvAfgJ0hTOD-iBg7LNW3OA/140.jpg</t>
+  </si>
+  <si>
     <t>http://www.ebay.com/itm/VINTAGE-LESLIE-ORGAN-SPEAKER-CABINET-MODEL-770-/142783280008</t>
   </si>
   <si>
+    <t>bedstuy872</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>173257976564</t>
   </si>
   <si>
     <t>Leslie 760 speaker and Hammond X-5 organ combo</t>
   </si>
   <si>
-    <t>2018-04-07T03:21:49.000Z</t>
-  </si>
-  <si>
-    <t>2018-04-14T03:21:49.000Z</t>
-  </si>
-  <si>
     <t>Hamburg,NY,USA</t>
   </si>
   <si>
+    <t>14075</t>
+  </si>
+  <si>
+    <t>http://thumbs1.ebaystatic.com/m/msDGps79PUtEL9h3R0v5QrQ/140.jpg</t>
+  </si>
+  <si>
     <t>http://www.ebay.com/itm/Leslie-760-speaker-and-Hammond-X-5-organ-combo-/173257976564</t>
   </si>
   <si>
+    <t>tkmaem</t>
+  </si>
+  <si>
+    <t>423</t>
+  </si>
+  <si>
     <t>172841790436</t>
   </si>
   <si>
     <t>Leslie Model 825 w/Pre-Amp 30ft original Cable Fully Operational Very Cool SRV</t>
   </si>
   <si>
-    <t>2017-08-28T11:44:18.000Z</t>
-  </si>
-  <si>
-    <t>2018-04-09T00:09:42.000Z</t>
-  </si>
-  <si>
     <t>Florence,SC,USA</t>
   </si>
   <si>
+    <t>29505</t>
+  </si>
+  <si>
+    <t>http://thumbs1.ebaystatic.com/m/mVtrQmgg_8kCZ8t_l-MdV9Q/140.jpg</t>
+  </si>
+  <si>
     <t>http://www.ebay.com/itm/Leslie-Model-825-w-Pre-Amp-30ft-original-Cable-Fully-Operational-Very-Cool-SRV-/172841790436</t>
+  </si>
+  <si>
+    <t>860buddy</t>
+  </si>
+  <si>
+    <t>1634</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -247,11 +304,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -549,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,7 +615,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,334 +661,430 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D2" t="n">
-        <v>495</v>
+        <v>750</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>43244.04601851852</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>43274.04601851852</v>
+      </c>
+      <c r="L2" t="n">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="n">
+        <v>495</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="n">
-        <v>91786</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="n">
-        <v>229</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>43260.88554398148</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>43270.88554398148</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2861</v>
-      </c>
-      <c r="O3" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D4" t="n">
-        <v>495</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>43232.738125</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>43256.83994212963</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" t="n">
-        <v>91786</v>
+        <v>46</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
       </c>
       <c r="O4" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="P4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" t="n">
         <v>495</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>43245.6600925926</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>43255.6600925926</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" t="n">
-        <v>2</v>
-      </c>
-      <c r="M5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N5" t="n">
-        <v>91786</v>
-      </c>
-      <c r="O5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
       <c r="D6" t="n">
         <v>500</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" t="s">
-        <v>47</v>
+        <v>25</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>43225.04082175926</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>43225.04747685185</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6" t="n">
-        <v>8108</v>
+        <v>58</v>
+      </c>
+      <c r="N6" t="s">
+        <v>59</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>60</v>
+      </c>
+      <c r="P6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D7" t="n">
         <v>510</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F7" t="n">
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K7" t="s">
-        <v>53</v>
+        <v>25</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>43197.14015046296</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>43204.14015046296</v>
       </c>
       <c r="L7" t="n">
         <v>28</v>
       </c>
       <c r="M7" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" t="n">
-        <v>14075</v>
+        <v>66</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
       </c>
       <c r="O7" t="s">
-        <v>55</v>
+        <v>68</v>
+      </c>
+      <c r="P7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>70</v>
+      </c>
+      <c r="R7" t="s">
+        <v>71</v>
+      </c>
+      <c r="S7" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" t="n">
         <v>500</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>42975.48909722222</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>43199.00673611111</v>
       </c>
       <c r="L8" t="n">
         <v>12</v>
       </c>
       <c r="M8" t="s">
-        <v>60</v>
-      </c>
-      <c r="N8" t="n">
-        <v>29505</v>
+        <v>74</v>
+      </c>
+      <c r="N8" t="s">
+        <v>75</v>
       </c>
       <c r="O8" t="s">
-        <v>61</v>
+        <v>76</v>
+      </c>
+      <c r="P8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" t="s">
+        <v>79</v>
+      </c>
+      <c r="S8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>